<commit_message>
Read track from file, no features
</commit_message>
<xml_diff>
--- a/resources/Sample_Track_File1.xlsx
+++ b/resources/Sample_Track_File1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\justc\Documents\School Stuff\Fall_2019\COE1186\Code\COE1186\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B01E308E-E9EE-4FCC-AF52-95EC6B8F2603}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B78C2D8-1F8D-440C-AC7A-E89A3D3938DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="80">
   <si>
     <t>Block Number</t>
   </si>
@@ -138,9 +138,6 @@
   </si>
   <si>
     <t>UNDERGROUND</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
   </si>
   <si>
     <t>ELEVATION (M)</t>
@@ -273,6 +270,9 @@
   </si>
   <si>
     <t>SWITCH (52-53; 52-66)</t>
+  </si>
+  <si>
+    <t>CUMULATIVE ELEVATION (M)</t>
   </si>
 </sst>
 </file>
@@ -1045,7 +1045,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B1" s="15"/>
       <c r="C1" s="15"/>
@@ -1074,11 +1074,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:L154"/>
+  <dimension ref="A1:L77"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G54" sqref="G54"/>
+      <pane ySplit="1" topLeftCell="A66" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K75" sqref="K75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -1112,16 +1112,16 @@
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>11</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J1" s="7" t="s">
-        <v>37</v>
+        <v>79</v>
       </c>
       <c r="K1" s="7"/>
     </row>
@@ -1322,7 +1322,7 @@
         <v>40</v>
       </c>
       <c r="G8" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I8" s="12">
         <f t="shared" si="0"/>
@@ -1383,7 +1383,7 @@
         <v>40</v>
       </c>
       <c r="G10" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I10" s="12">
         <f t="shared" si="0"/>
@@ -1560,7 +1560,7 @@
         <v>40</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I16" s="12">
         <f t="shared" si="0"/>
@@ -1592,7 +1592,7 @@
         <v>40</v>
       </c>
       <c r="G17" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I17" s="12">
         <f t="shared" si="0"/>
@@ -1741,7 +1741,7 @@
         <v>55</v>
       </c>
       <c r="G22" s="11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I22" s="12">
         <f t="shared" si="0"/>
@@ -1863,7 +1863,7 @@
         <v>70</v>
       </c>
       <c r="G26" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I26" s="12">
         <f t="shared" si="0"/>
@@ -1927,7 +1927,7 @@
         <v>70</v>
       </c>
       <c r="G28" s="11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I28" s="12">
         <f t="shared" si="0"/>
@@ -2087,7 +2087,7 @@
         <v>70</v>
       </c>
       <c r="G33" s="11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I33" s="12">
         <f t="shared" si="0"/>
@@ -2183,7 +2183,7 @@
         <v>70</v>
       </c>
       <c r="G36" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I36" s="12">
         <f t="shared" si="0"/>
@@ -2279,7 +2279,7 @@
         <v>70</v>
       </c>
       <c r="G39" s="11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I39" s="12">
         <f t="shared" si="0"/>
@@ -2439,7 +2439,7 @@
         <v>70</v>
       </c>
       <c r="G44" s="11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I44" s="12">
         <f t="shared" si="0"/>
@@ -2503,7 +2503,7 @@
         <v>70</v>
       </c>
       <c r="G46" s="11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I46" s="12">
         <f t="shared" si="0"/>
@@ -2567,7 +2567,7 @@
         <v>70</v>
       </c>
       <c r="G48" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I48" s="12">
         <f t="shared" si="0"/>
@@ -2599,7 +2599,7 @@
         <v>70</v>
       </c>
       <c r="G49" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I49" s="12">
         <f t="shared" si="0"/>
@@ -2718,7 +2718,7 @@
         <v>55</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I53" s="12">
         <f t="shared" si="0"/>
@@ -2953,7 +2953,7 @@
         <v>55</v>
       </c>
       <c r="G61" s="11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I61" s="12">
         <f t="shared" si="0"/>
@@ -3236,7 +3236,7 @@
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A71" s="3" t="str">
-        <f t="shared" ref="A71:A134" si="5">A70</f>
+        <f t="shared" ref="A71:A77" si="5">A70</f>
         <v>Red</v>
       </c>
       <c r="B71" s="3" t="s">
@@ -3457,544 +3457,6 @@
         <f t="shared" si="4"/>
         <v>-1.2410000000000001</v>
       </c>
-    </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A78" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C78" s="5"/>
-    </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A79" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C79" s="5"/>
-    </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A80" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C80" s="5"/>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A81" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C81" s="5"/>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A82" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C82" s="5"/>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A83" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C83" s="5"/>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A84" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C84" s="5"/>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A85" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C85" s="5"/>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A86" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C86" s="5"/>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A87" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C87" s="5"/>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A88" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C88" s="5"/>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A89" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C89" s="5"/>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A90" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C90" s="5"/>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A91" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C91" s="5"/>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A92" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C92" s="5"/>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A93" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C93" s="5"/>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A94" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C94" s="5"/>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A95" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C95" s="5"/>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A96" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C96" s="5"/>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A97" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C97" s="5"/>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A98" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C98" s="5"/>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A99" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C99" s="5"/>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A100" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C100" s="5"/>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A101" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C101" s="5"/>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A102" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C102" s="5"/>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A103" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C103" s="5"/>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A104" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C104" s="5"/>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A105" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C105" s="5"/>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A106" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C106" s="5"/>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A107" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C107" s="5"/>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A108" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C108" s="5"/>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A109" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C109" s="5"/>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A110" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C110" s="5"/>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A111" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C111" s="5"/>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A112" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C112" s="5"/>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A113" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C113" s="5"/>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A114" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C114" s="5"/>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A115" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C115" s="5"/>
-    </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A116" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C116" s="5"/>
-    </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A117" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C117" s="5"/>
-    </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A118" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C118" s="5"/>
-    </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A119" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C119" s="5"/>
-    </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A120" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C120" s="5"/>
-    </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A121" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C121" s="5"/>
-    </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A122" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C122" s="5"/>
-    </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A123" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C123" s="5"/>
-    </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A124" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C124" s="5"/>
-    </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A125" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C125" s="5"/>
-    </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A126" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C126" s="5"/>
-    </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A127" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C127" s="5"/>
-    </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A128" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C128" s="5"/>
-    </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A129" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C129" s="5"/>
-    </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A130" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C130" s="5"/>
-    </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A131" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C131" s="5"/>
-    </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A132" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C132" s="5"/>
-    </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A133" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C133" s="5"/>
-    </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A134" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C134" s="5"/>
-    </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A135" s="3" t="str">
-        <f t="shared" ref="A135:A154" si="6">A134</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C135" s="5"/>
-    </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A136" s="3" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C136" s="5"/>
-    </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A137" s="3" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C137" s="5"/>
-    </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A138" s="3" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C138" s="5"/>
-    </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A139" s="3" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C139" s="5"/>
-    </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A140" s="3" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C140" s="5"/>
-    </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A141" s="3" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C141" s="5"/>
-    </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A142" s="3" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C142" s="5"/>
-    </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A143" s="3" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C143" s="5"/>
-    </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A144" s="3" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C144" s="5"/>
-    </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A145" s="3" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C145" s="5"/>
-    </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A146" s="3" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C146" s="5"/>
-    </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A147" s="3" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C147" s="5"/>
-    </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A148" s="3" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C148" s="5"/>
-    </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A149" s="3" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C149" s="5"/>
-    </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A150" s="3" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C150" s="5"/>
-    </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A151" s="3" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C151" s="5"/>
-    </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A152" s="3" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C152" s="5"/>
-    </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A153" s="3" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C153" s="5"/>
-    </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A154" s="3" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C154" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4042,16 +3504,16 @@
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>11</v>
       </c>
       <c r="I1" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="J1" s="7" t="s">
         <v>36</v>
-      </c>
-      <c r="J1" s="7" t="s">
-        <v>37</v>
       </c>
       <c r="K1" s="7"/>
     </row>
@@ -4105,7 +3567,7 @@
         <v>55</v>
       </c>
       <c r="G3" s="11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I3" s="3">
         <f t="shared" ref="I3:I66" si="0">E3*D3/100</f>
@@ -4314,7 +3776,7 @@
         <v>55</v>
       </c>
       <c r="G10" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I10" s="3">
         <f t="shared" si="0"/>
@@ -4404,7 +3866,7 @@
         <v>55</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I13" s="3">
         <f t="shared" si="0"/>
@@ -4613,7 +4075,7 @@
         <v>60</v>
       </c>
       <c r="G20" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I20" s="3">
         <f t="shared" si="0"/>
@@ -4703,7 +4165,7 @@
         <v>70</v>
       </c>
       <c r="G23" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I23" s="3">
         <f t="shared" si="0"/>
@@ -4909,7 +4371,7 @@
         <v>70</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I30" s="3">
         <f t="shared" si="0"/>
@@ -4970,7 +4432,7 @@
         <v>70</v>
       </c>
       <c r="G32" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I32" s="3">
         <f t="shared" si="0"/>
@@ -5214,7 +4676,7 @@
         <v>70</v>
       </c>
       <c r="G40" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I40" s="3">
         <f t="shared" si="0"/>
@@ -5502,7 +4964,7 @@
         <v>70</v>
       </c>
       <c r="G49" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I49" s="3">
         <f t="shared" si="0"/>
@@ -5790,7 +5252,7 @@
         <v>70</v>
       </c>
       <c r="G58" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I58" s="3">
         <f t="shared" si="0"/>
@@ -5822,7 +5284,7 @@
         <v>60</v>
       </c>
       <c r="G59" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I59" s="3">
         <f t="shared" si="0"/>
@@ -5941,7 +5403,7 @@
         <v>60</v>
       </c>
       <c r="G63" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I63" s="3">
         <f t="shared" si="0"/>
@@ -6031,7 +5493,7 @@
         <v>70</v>
       </c>
       <c r="G66" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I66" s="3">
         <f t="shared" si="0"/>
@@ -6266,7 +5728,7 @@
         <v>60</v>
       </c>
       <c r="G74" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I74" s="3">
         <f t="shared" si="3"/>
@@ -6356,7 +5818,7 @@
         <v>60</v>
       </c>
       <c r="G77" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I77" s="3">
         <f t="shared" si="3"/>
@@ -6388,7 +5850,7 @@
         <v>70</v>
       </c>
       <c r="G78" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I78" s="3">
         <f t="shared" ref="I78:I109" si="6">E78*D78/100</f>
@@ -6652,7 +6114,7 @@
         <v>55</v>
       </c>
       <c r="G87" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I87" s="3">
         <f t="shared" si="6"/>
@@ -6713,7 +6175,7 @@
         <v>55</v>
       </c>
       <c r="G89" s="11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I89" s="3">
         <f t="shared" si="6"/>
@@ -6948,7 +6410,7 @@
         <v>55</v>
       </c>
       <c r="G97" s="11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I97" s="3">
         <f t="shared" si="6"/>
@@ -7346,7 +6808,7 @@
         <v>Green</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C111" s="5">
         <v>110</v>
@@ -7375,7 +6837,7 @@
         <v>Green</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C112" s="3">
         <v>111</v>
@@ -7404,7 +6866,7 @@
         <v>Green</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C113" s="3">
         <v>112</v>
@@ -7433,7 +6895,7 @@
         <v>Green</v>
       </c>
       <c r="B114" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C114" s="3">
         <v>113</v>
@@ -7462,7 +6924,7 @@
         <v>Green</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C115" s="5">
         <v>114</v>
@@ -7496,7 +6958,7 @@
         <v>Green</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C116" s="3">
         <v>115</v>
@@ -7525,7 +6987,7 @@
         <v>Green</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C117" s="3">
         <v>116</v>
@@ -7554,7 +7016,7 @@
         <v>Green</v>
       </c>
       <c r="B118" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C118" s="3">
         <v>117</v>
@@ -7583,7 +7045,7 @@
         <v>Green</v>
       </c>
       <c r="B119" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C119" s="5">
         <v>118</v>
@@ -7612,7 +7074,7 @@
         <v>Green</v>
       </c>
       <c r="B120" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C120" s="3">
         <v>119</v>
@@ -7641,7 +7103,7 @@
         <v>Green</v>
       </c>
       <c r="B121" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C121" s="3">
         <v>120</v>
@@ -7670,7 +7132,7 @@
         <v>Green</v>
       </c>
       <c r="B122" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C122" s="3">
         <v>121</v>
@@ -7699,7 +7161,7 @@
         <v>Green</v>
       </c>
       <c r="B123" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C123" s="5">
         <v>122</v>
@@ -7731,7 +7193,7 @@
         <v>Green</v>
       </c>
       <c r="B124" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C124" s="3">
         <v>123</v>
@@ -7764,7 +7226,7 @@
         <v>Green</v>
       </c>
       <c r="B125" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C125" s="3">
         <v>124</v>
@@ -7796,7 +7258,7 @@
         <v>Green</v>
       </c>
       <c r="B126" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C126" s="3">
         <v>125</v>
@@ -7828,7 +7290,7 @@
         <v>Green</v>
       </c>
       <c r="B127" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C127" s="5">
         <v>126</v>
@@ -7860,7 +7322,7 @@
         <v>Green</v>
       </c>
       <c r="B128" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C128" s="3">
         <v>127</v>
@@ -7892,7 +7354,7 @@
         <v>Green</v>
       </c>
       <c r="B129" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C129" s="3">
         <v>128</v>
@@ -7924,7 +7386,7 @@
         <v>Green</v>
       </c>
       <c r="B130" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C130" s="3">
         <v>129</v>
@@ -7956,7 +7418,7 @@
         <v>Green</v>
       </c>
       <c r="B131" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C131" s="5">
         <v>130</v>
@@ -7988,7 +7450,7 @@
         <v>Green</v>
       </c>
       <c r="B132" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C132" s="3">
         <v>131</v>
@@ -8020,7 +7482,7 @@
         <v>Green</v>
       </c>
       <c r="B133" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C133" s="3">
         <v>132</v>
@@ -8053,7 +7515,7 @@
         <v>Green</v>
       </c>
       <c r="B134" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C134" s="3">
         <v>133</v>
@@ -8085,7 +7547,7 @@
         <v>Green</v>
       </c>
       <c r="B135" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C135" s="5">
         <v>134</v>
@@ -8117,7 +7579,7 @@
         <v>Green</v>
       </c>
       <c r="B136" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C136" s="3">
         <v>135</v>
@@ -8149,7 +7611,7 @@
         <v>Green</v>
       </c>
       <c r="B137" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C137" s="3">
         <v>136</v>
@@ -8181,7 +7643,7 @@
         <v>Green</v>
       </c>
       <c r="B138" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C138" s="3">
         <v>137</v>
@@ -8213,7 +7675,7 @@
         <v>Green</v>
       </c>
       <c r="B139" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C139" s="5">
         <v>138</v>
@@ -8245,7 +7707,7 @@
         <v>Green</v>
       </c>
       <c r="B140" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C140" s="3">
         <v>139</v>
@@ -8277,7 +7739,7 @@
         <v>Green</v>
       </c>
       <c r="B141" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C141" s="3">
         <v>140</v>
@@ -8309,7 +7771,7 @@
         <v>Green</v>
       </c>
       <c r="B142" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C142" s="3">
         <v>141</v>
@@ -8342,7 +7804,7 @@
         <v>Green</v>
       </c>
       <c r="B143" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C143" s="5">
         <v>142</v>
@@ -8374,7 +7836,7 @@
         <v>Green</v>
       </c>
       <c r="B144" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C144" s="3">
         <v>143</v>
@@ -8406,7 +7868,7 @@
         <v>Green</v>
       </c>
       <c r="B145" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C145" s="3">
         <v>144</v>
@@ -8435,7 +7897,7 @@
         <v>Green</v>
       </c>
       <c r="B146" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C146" s="3">
         <v>145</v>
@@ -8464,7 +7926,7 @@
         <v>Green</v>
       </c>
       <c r="B147" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C147" s="5">
         <v>146</v>
@@ -8493,7 +7955,7 @@
         <v>Green</v>
       </c>
       <c r="B148" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C148" s="3">
         <v>147</v>
@@ -8522,7 +7984,7 @@
         <v>Green</v>
       </c>
       <c r="B149" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C149" s="3">
         <v>148</v>
@@ -8552,7 +8014,7 @@
         <v>Green</v>
       </c>
       <c r="B150" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C150" s="3">
         <v>149</v>
@@ -8581,7 +8043,7 @@
         <v>Green</v>
       </c>
       <c r="B151" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C151" s="5">
         <v>150</v>
@@ -8613,7 +8075,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="K51" sqref="K51"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Read track from file, no switches/branches
</commit_message>
<xml_diff>
--- a/resources/Sample_Track_File1.xlsx
+++ b/resources/Sample_Track_File1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\justc\Documents\School Stuff\Fall_2019\COE1186\Code\COE1186\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B78C2D8-1F8D-440C-AC7A-E89A3D3938DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CC1C86C-8420-479C-A6A4-A5D85E51734B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -152,15 +152,6 @@
     <t>STATION: HERRON AVE</t>
   </si>
   <si>
-    <t>STATION;     STEEL PLAZA; UNDERGROUND</t>
-  </si>
-  <si>
-    <t>STATION; STATION SQUARE</t>
-  </si>
-  <si>
-    <t>STATION; SOUTH HILLS JUNCTION</t>
-  </si>
-  <si>
     <t>Speed Limit (Km/Hr)</t>
   </si>
   <si>
@@ -215,9 +206,6 @@
     <t>STATION; OVERBROOK; UNDERGROUND</t>
   </si>
   <si>
-    <t>STATION; SWISSVILLE</t>
-  </si>
-  <si>
     <t>RAILWAY CROSSING</t>
   </si>
   <si>
@@ -251,9 +239,6 @@
     <t>SWITCH (15-16; 1-16)</t>
   </si>
   <si>
-    <t>STATION; PENN STATION; UNDERGROUND</t>
-  </si>
-  <si>
     <t>SWITCH (27-28; 27-76); UNDERGROUND</t>
   </si>
   <si>
@@ -266,13 +251,28 @@
     <t>SWITCH (43-44; 43-67); UNDERGROUND</t>
   </si>
   <si>
-    <t>STATION; FIRST AVE; UNDERGROUND</t>
-  </si>
-  <si>
     <t>SWITCH (52-53; 52-66)</t>
   </si>
   <si>
     <t>CUMULATIVE ELEVATION (M)</t>
+  </si>
+  <si>
+    <t>STATION: STATION SQUARE</t>
+  </si>
+  <si>
+    <t>STATION: FIRST AVE; UNDERGROUND</t>
+  </si>
+  <si>
+    <t>STATION: SOUTH HILLS JUNCTION</t>
+  </si>
+  <si>
+    <t>STATION: STEEL PLAZA; UNDERGROUND</t>
+  </si>
+  <si>
+    <t>STATION: PENN STATION; UNDERGROUND</t>
+  </si>
+  <si>
+    <t>STATION: SWISSVILLE</t>
   </si>
 </sst>
 </file>
@@ -1045,7 +1045,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="14" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B1" s="15"/>
       <c r="C1" s="15"/>
@@ -1077,8 +1077,8 @@
   <dimension ref="A1:L77"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A66" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K75" sqref="K75"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -1090,7 +1090,9 @@
     <col min="5" max="5" width="10.54296875" style="3" customWidth="1"/>
     <col min="6" max="6" width="13.26953125" style="3" customWidth="1"/>
     <col min="7" max="7" width="43" style="3" customWidth="1"/>
-    <col min="8" max="12" width="8.81640625" style="1"/>
+    <col min="8" max="9" width="8.81640625" style="1"/>
+    <col min="10" max="10" width="8.6328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="8.81640625" style="1"/>
     <col min="13" max="13" width="11.453125" style="1" customWidth="1"/>
     <col min="14" max="16384" width="8.81640625" style="1"/>
   </cols>
@@ -1112,7 +1114,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>11</v>
@@ -1121,7 +1123,7 @@
         <v>35</v>
       </c>
       <c r="J1" s="7" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="K1" s="7"/>
     </row>
@@ -1383,7 +1385,7 @@
         <v>40</v>
       </c>
       <c r="G10" s="11" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="I10" s="12">
         <f t="shared" si="0"/>
@@ -1560,7 +1562,7 @@
         <v>40</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="I16" s="12">
         <f t="shared" si="0"/>
@@ -1741,7 +1743,7 @@
         <v>55</v>
       </c>
       <c r="G22" s="11" t="s">
-        <v>60</v>
+        <v>79</v>
       </c>
       <c r="I22" s="12">
         <f t="shared" si="0"/>
@@ -1863,7 +1865,7 @@
         <v>70</v>
       </c>
       <c r="G26" s="11" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="I26" s="12">
         <f t="shared" si="0"/>
@@ -1927,7 +1929,7 @@
         <v>70</v>
       </c>
       <c r="G28" s="11" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="I28" s="12">
         <f t="shared" si="0"/>
@@ -2087,7 +2089,7 @@
         <v>70</v>
       </c>
       <c r="G33" s="11" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="I33" s="12">
         <f t="shared" si="0"/>
@@ -2183,7 +2185,7 @@
         <v>70</v>
       </c>
       <c r="G36" s="11" t="s">
-        <v>39</v>
+        <v>77</v>
       </c>
       <c r="I36" s="12">
         <f t="shared" si="0"/>
@@ -2279,7 +2281,7 @@
         <v>70</v>
       </c>
       <c r="G39" s="11" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="I39" s="12">
         <f t="shared" si="0"/>
@@ -2439,7 +2441,7 @@
         <v>70</v>
       </c>
       <c r="G44" s="11" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="I44" s="12">
         <f t="shared" si="0"/>
@@ -2503,7 +2505,7 @@
         <v>70</v>
       </c>
       <c r="G46" s="11" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="I46" s="12">
         <f t="shared" si="0"/>
@@ -2567,7 +2569,7 @@
         <v>70</v>
       </c>
       <c r="G48" s="11" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="I48" s="12">
         <f t="shared" si="0"/>
@@ -2599,7 +2601,7 @@
         <v>70</v>
       </c>
       <c r="G49" s="11" t="s">
-        <v>40</v>
+        <v>74</v>
       </c>
       <c r="I49" s="12">
         <f t="shared" si="0"/>
@@ -2718,7 +2720,7 @@
         <v>55</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="I53" s="12">
         <f t="shared" si="0"/>
@@ -2953,7 +2955,7 @@
         <v>55</v>
       </c>
       <c r="G61" s="11" t="s">
-        <v>41</v>
+        <v>76</v>
       </c>
       <c r="I61" s="12">
         <f t="shared" si="0"/>
@@ -3469,7 +3471,7 @@
   <dimension ref="A1:L151"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A94" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A107" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="G88" sqref="G88"/>
     </sheetView>
   </sheetViews>
@@ -3504,7 +3506,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>11</v>
@@ -3567,7 +3569,7 @@
         <v>55</v>
       </c>
       <c r="G3" s="11" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="I3" s="3">
         <f t="shared" ref="I3:I66" si="0">E3*D3/100</f>
@@ -3776,7 +3778,7 @@
         <v>55</v>
       </c>
       <c r="G10" s="11" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="I10" s="3">
         <f t="shared" si="0"/>
@@ -3866,7 +3868,7 @@
         <v>55</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="I13" s="3">
         <f t="shared" si="0"/>
@@ -4075,7 +4077,7 @@
         <v>60</v>
       </c>
       <c r="G20" s="11" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="I20" s="3">
         <f t="shared" si="0"/>
@@ -4165,7 +4167,7 @@
         <v>70</v>
       </c>
       <c r="G23" s="11" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="I23" s="3">
         <f t="shared" si="0"/>
@@ -4371,7 +4373,7 @@
         <v>70</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="I30" s="3">
         <f t="shared" si="0"/>
@@ -4432,7 +4434,7 @@
         <v>70</v>
       </c>
       <c r="G32" s="11" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="I32" s="3">
         <f t="shared" si="0"/>
@@ -4676,7 +4678,7 @@
         <v>70</v>
       </c>
       <c r="G40" s="11" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="I40" s="3">
         <f t="shared" si="0"/>
@@ -4964,7 +4966,7 @@
         <v>70</v>
       </c>
       <c r="G49" s="11" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="I49" s="3">
         <f t="shared" si="0"/>
@@ -5252,7 +5254,7 @@
         <v>70</v>
       </c>
       <c r="G58" s="11" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="I58" s="3">
         <f t="shared" si="0"/>
@@ -5284,7 +5286,7 @@
         <v>60</v>
       </c>
       <c r="G59" s="11" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="I59" s="3">
         <f t="shared" si="0"/>
@@ -5403,7 +5405,7 @@
         <v>60</v>
       </c>
       <c r="G63" s="11" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="I63" s="3">
         <f t="shared" si="0"/>
@@ -5493,7 +5495,7 @@
         <v>70</v>
       </c>
       <c r="G66" s="11" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="I66" s="3">
         <f t="shared" si="0"/>
@@ -5728,7 +5730,7 @@
         <v>60</v>
       </c>
       <c r="G74" s="11" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="I74" s="3">
         <f t="shared" si="3"/>
@@ -5818,7 +5820,7 @@
         <v>60</v>
       </c>
       <c r="G77" s="3" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="I77" s="3">
         <f t="shared" si="3"/>
@@ -5850,7 +5852,7 @@
         <v>70</v>
       </c>
       <c r="G78" s="11" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="I78" s="3">
         <f t="shared" ref="I78:I109" si="6">E78*D78/100</f>
@@ -6114,7 +6116,7 @@
         <v>55</v>
       </c>
       <c r="G87" s="3" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="I87" s="3">
         <f t="shared" si="6"/>
@@ -6175,7 +6177,7 @@
         <v>55</v>
       </c>
       <c r="G89" s="11" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="I89" s="3">
         <f t="shared" si="6"/>
@@ -6410,7 +6412,7 @@
         <v>55</v>
       </c>
       <c r="G97" s="11" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="I97" s="3">
         <f t="shared" si="6"/>
@@ -6653,7 +6655,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="106" spans="1:10" ht="31" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A106" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -6808,7 +6810,7 @@
         <v>Green</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C111" s="5">
         <v>110</v>
@@ -6837,7 +6839,7 @@
         <v>Green</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C112" s="3">
         <v>111</v>
@@ -6866,7 +6868,7 @@
         <v>Green</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C113" s="3">
         <v>112</v>
@@ -6895,7 +6897,7 @@
         <v>Green</v>
       </c>
       <c r="B114" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C114" s="3">
         <v>113</v>
@@ -6924,7 +6926,7 @@
         <v>Green</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C115" s="5">
         <v>114</v>
@@ -6958,7 +6960,7 @@
         <v>Green</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C116" s="3">
         <v>115</v>
@@ -6987,7 +6989,7 @@
         <v>Green</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C117" s="3">
         <v>116</v>
@@ -7016,7 +7018,7 @@
         <v>Green</v>
       </c>
       <c r="B118" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C118" s="3">
         <v>117</v>
@@ -7045,7 +7047,7 @@
         <v>Green</v>
       </c>
       <c r="B119" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C119" s="5">
         <v>118</v>
@@ -7074,7 +7076,7 @@
         <v>Green</v>
       </c>
       <c r="B120" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C120" s="3">
         <v>119</v>
@@ -7103,7 +7105,7 @@
         <v>Green</v>
       </c>
       <c r="B121" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C121" s="3">
         <v>120</v>
@@ -7132,7 +7134,7 @@
         <v>Green</v>
       </c>
       <c r="B122" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C122" s="3">
         <v>121</v>
@@ -7161,7 +7163,7 @@
         <v>Green</v>
       </c>
       <c r="B123" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C123" s="5">
         <v>122</v>
@@ -7193,7 +7195,7 @@
         <v>Green</v>
       </c>
       <c r="B124" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C124" s="3">
         <v>123</v>
@@ -7226,7 +7228,7 @@
         <v>Green</v>
       </c>
       <c r="B125" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C125" s="3">
         <v>124</v>
@@ -7258,7 +7260,7 @@
         <v>Green</v>
       </c>
       <c r="B126" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C126" s="3">
         <v>125</v>
@@ -7290,7 +7292,7 @@
         <v>Green</v>
       </c>
       <c r="B127" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C127" s="5">
         <v>126</v>
@@ -7322,7 +7324,7 @@
         <v>Green</v>
       </c>
       <c r="B128" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C128" s="3">
         <v>127</v>
@@ -7354,7 +7356,7 @@
         <v>Green</v>
       </c>
       <c r="B129" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C129" s="3">
         <v>128</v>
@@ -7386,7 +7388,7 @@
         <v>Green</v>
       </c>
       <c r="B130" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C130" s="3">
         <v>129</v>
@@ -7418,7 +7420,7 @@
         <v>Green</v>
       </c>
       <c r="B131" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C131" s="5">
         <v>130</v>
@@ -7450,7 +7452,7 @@
         <v>Green</v>
       </c>
       <c r="B132" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C132" s="3">
         <v>131</v>
@@ -7482,7 +7484,7 @@
         <v>Green</v>
       </c>
       <c r="B133" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C133" s="3">
         <v>132</v>
@@ -7515,7 +7517,7 @@
         <v>Green</v>
       </c>
       <c r="B134" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C134" s="3">
         <v>133</v>
@@ -7547,7 +7549,7 @@
         <v>Green</v>
       </c>
       <c r="B135" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C135" s="5">
         <v>134</v>
@@ -7579,7 +7581,7 @@
         <v>Green</v>
       </c>
       <c r="B136" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C136" s="3">
         <v>135</v>
@@ -7611,7 +7613,7 @@
         <v>Green</v>
       </c>
       <c r="B137" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C137" s="3">
         <v>136</v>
@@ -7643,7 +7645,7 @@
         <v>Green</v>
       </c>
       <c r="B138" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C138" s="3">
         <v>137</v>
@@ -7675,7 +7677,7 @@
         <v>Green</v>
       </c>
       <c r="B139" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C139" s="5">
         <v>138</v>
@@ -7707,7 +7709,7 @@
         <v>Green</v>
       </c>
       <c r="B140" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C140" s="3">
         <v>139</v>
@@ -7739,7 +7741,7 @@
         <v>Green</v>
       </c>
       <c r="B141" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C141" s="3">
         <v>140</v>
@@ -7771,7 +7773,7 @@
         <v>Green</v>
       </c>
       <c r="B142" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C142" s="3">
         <v>141</v>
@@ -7804,7 +7806,7 @@
         <v>Green</v>
       </c>
       <c r="B143" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C143" s="5">
         <v>142</v>
@@ -7836,7 +7838,7 @@
         <v>Green</v>
       </c>
       <c r="B144" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C144" s="3">
         <v>143</v>
@@ -7868,7 +7870,7 @@
         <v>Green</v>
       </c>
       <c r="B145" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C145" s="3">
         <v>144</v>
@@ -7897,7 +7899,7 @@
         <v>Green</v>
       </c>
       <c r="B146" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C146" s="3">
         <v>145</v>
@@ -7926,7 +7928,7 @@
         <v>Green</v>
       </c>
       <c r="B147" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C147" s="5">
         <v>146</v>
@@ -7955,7 +7957,7 @@
         <v>Green</v>
       </c>
       <c r="B148" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C148" s="3">
         <v>147</v>
@@ -7984,7 +7986,7 @@
         <v>Green</v>
       </c>
       <c r="B149" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C149" s="3">
         <v>148</v>
@@ -8014,7 +8016,7 @@
         <v>Green</v>
       </c>
       <c r="B150" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C150" s="3">
         <v>149</v>
@@ -8043,7 +8045,7 @@
         <v>Green</v>
       </c>
       <c r="B151" s="3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C151" s="5">
         <v>150</v>

</xml_diff>